<commit_message>
Added data provider for try editor positive and negative
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,10 +4,11 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="LoginCredentials" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="RegisterPage" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="PracticeQns" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="TryEditor" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="LinkedListTopics" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="TreePage" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="RegisterPage" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="PracticeQns" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="TryEditor" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="LinkedListTopics" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="64">
   <si>
     <t>username</t>
   </si>
@@ -45,6 +46,21 @@
   </si>
   <si>
     <t>Dre@m</t>
+  </si>
+  <si>
+    <t>TestScenario</t>
+  </si>
+  <si>
+    <t>Priority1</t>
+  </si>
+  <si>
+    <t>Data Structures-Introduction</t>
+  </si>
+  <si>
+    <t>Priority2</t>
+  </si>
+  <si>
+    <t>Time Complexity</t>
   </si>
   <si>
     <t>password confirmation</t>
@@ -152,6 +168,21 @@
     <t>print 1234</t>
   </si>
   <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>print hello</t>
+  </si>
+  <si>
+    <t>NameError: name 'hello' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>aer234@$</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad token T_OP on line 1</t>
+  </si>
+  <si>
     <t>link</t>
   </si>
   <si>
@@ -211,20 +242,18 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -253,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -263,27 +292,39 @@
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -311,6 +352,10 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -7511,6 +7556,141 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="13.38"/>
+    <col customWidth="1" min="2" max="2" width="19.13"/>
+    <col customWidth="1" min="3" max="3" width="19.75"/>
+    <col customWidth="1" min="4" max="4" width="29.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="D4" s="8"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
@@ -7526,125 +7706,125 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="5" t="s">
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="5" t="s">
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="5" t="s">
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>26</v>
       </c>
+      <c r="B5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
+      <c r="A6" s="9" t="s">
+        <v>20</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>28</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9" t="s">
+        <v>28</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>13</v>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>13</v>
+      <c r="C10" s="10" t="s">
+        <v>18</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>17</v>
+      <c r="D10" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1"/>
@@ -8638,20 +8818,14 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="B2"/>
-    <hyperlink r:id="rId2" ref="C2"/>
-    <hyperlink r:id="rId3" ref="B10"/>
-    <hyperlink r:id="rId4" ref="C10"/>
-  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -8668,11 +8842,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>24</v>
+      <c r="A1" s="11" t="s">
+        <v>29</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>25</v>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -8700,11 +8874,11 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>26</v>
+      <c r="A2" s="12" t="s">
+        <v>31</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>27</v>
+      <c r="B2" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -8732,11 +8906,11 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>28</v>
+      <c r="A3" s="12" t="s">
+        <v>33</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>29</v>
+      <c r="B3" s="11" t="s">
+        <v>34</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -8764,8 +8938,8 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -8792,10 +8966,10 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="8" t="s">
-        <v>30</v>
+      <c r="A5" s="12" t="s">
+        <v>35</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="11">
         <v>2.0</v>
       </c>
       <c r="C5" s="2"/>
@@ -8824,10 +8998,10 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="8" t="s">
-        <v>31</v>
+      <c r="A6" s="12" t="s">
+        <v>36</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="11">
         <v>3.0</v>
       </c>
       <c r="C6" s="2"/>
@@ -8856,10 +9030,10 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>32</v>
+      <c r="A7" s="15" t="s">
+        <v>37</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="11">
         <v>2.0</v>
       </c>
       <c r="C7" s="2"/>
@@ -8888,10 +9062,10 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="11" t="s">
-        <v>33</v>
+      <c r="A8" s="15" t="s">
+        <v>38</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="11">
         <v>1.0</v>
       </c>
       <c r="C8" s="2"/>
@@ -8920,11 +9094,11 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="11" t="s">
-        <v>34</v>
+      <c r="A9" s="15" t="s">
+        <v>39</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>35</v>
+      <c r="B9" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -8952,11 +9126,11 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="11" t="s">
-        <v>36</v>
+      <c r="A10" s="15" t="s">
+        <v>41</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>37</v>
+      <c r="B10" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -8984,11 +9158,11 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>26</v>
+      <c r="A11" s="12" t="s">
+        <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>38</v>
+      <c r="B11" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -9016,11 +9190,11 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>30</v>
+      <c r="A12" s="12" t="s">
+        <v>35</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>38</v>
+      <c r="B12" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -9048,11 +9222,11 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="11" t="s">
-        <v>32</v>
+      <c r="A13" s="15" t="s">
+        <v>37</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>39</v>
+      <c r="B13" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -9080,11 +9254,11 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
-        <v>34</v>
+      <c r="A14" s="15" t="s">
+        <v>39</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>40</v>
+      <c r="B14" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -9112,8 +9286,8 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -9140,8 +9314,8 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -9168,8 +9342,8 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -9196,8 +9370,8 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -9224,8 +9398,8 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -9252,808 +9426,808 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="16"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="16"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="16"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="16"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="10"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="14"/>
+      <c r="B24" s="16"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="10"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="16"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="10"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="14"/>
+      <c r="B26" s="16"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="10"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="16"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="16"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="10"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="16"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="10"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="16"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="10"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="14"/>
+      <c r="B31" s="16"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="10"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="16"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="10"/>
-      <c r="B33" s="12"/>
+      <c r="A33" s="14"/>
+      <c r="B33" s="16"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="10"/>
-      <c r="B34" s="12"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="16"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="10"/>
-      <c r="B35" s="12"/>
+      <c r="A35" s="14"/>
+      <c r="B35" s="16"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="10"/>
-      <c r="B36" s="12"/>
+      <c r="A36" s="14"/>
+      <c r="B36" s="16"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="10"/>
-      <c r="B37" s="12"/>
+      <c r="A37" s="14"/>
+      <c r="B37" s="16"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="10"/>
-      <c r="B38" s="12"/>
+      <c r="A38" s="14"/>
+      <c r="B38" s="16"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="10"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="14"/>
+      <c r="B39" s="16"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="10"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="14"/>
+      <c r="B40" s="16"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="10"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="16"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="10"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="14"/>
+      <c r="B42" s="16"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="10"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="14"/>
+      <c r="B43" s="16"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="10"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="14"/>
+      <c r="B44" s="16"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="10"/>
-      <c r="B45" s="12"/>
+      <c r="A45" s="14"/>
+      <c r="B45" s="16"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="10"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="14"/>
+      <c r="B46" s="16"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="10"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="14"/>
+      <c r="B47" s="16"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="10"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="16"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="10"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="14"/>
+      <c r="B49" s="16"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="10"/>
-      <c r="B50" s="12"/>
+      <c r="A50" s="14"/>
+      <c r="B50" s="16"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="10"/>
-      <c r="B51" s="12"/>
+      <c r="A51" s="14"/>
+      <c r="B51" s="16"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="10"/>
-      <c r="B52" s="12"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="16"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="10"/>
-      <c r="B53" s="12"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="16"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="10"/>
-      <c r="B54" s="12"/>
+      <c r="A54" s="14"/>
+      <c r="B54" s="16"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="10"/>
-      <c r="B55" s="12"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="16"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="10"/>
-      <c r="B56" s="12"/>
+      <c r="A56" s="14"/>
+      <c r="B56" s="16"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="10"/>
-      <c r="B57" s="12"/>
+      <c r="A57" s="14"/>
+      <c r="B57" s="16"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="10"/>
-      <c r="B58" s="12"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="16"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="10"/>
-      <c r="B59" s="12"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="16"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="10"/>
-      <c r="B60" s="12"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="16"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="10"/>
-      <c r="B61" s="12"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="16"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="10"/>
-      <c r="B62" s="12"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="16"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="10"/>
-      <c r="B63" s="12"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="16"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="10"/>
-      <c r="B64" s="12"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="16"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="10"/>
-      <c r="B65" s="12"/>
+      <c r="A65" s="14"/>
+      <c r="B65" s="16"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="10"/>
-      <c r="B66" s="12"/>
+      <c r="A66" s="14"/>
+      <c r="B66" s="16"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="10"/>
-      <c r="B67" s="12"/>
+      <c r="A67" s="14"/>
+      <c r="B67" s="16"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="10"/>
-      <c r="B68" s="12"/>
+      <c r="A68" s="14"/>
+      <c r="B68" s="16"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="10"/>
-      <c r="B69" s="12"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="16"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="10"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="16"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="10"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="14"/>
+      <c r="B71" s="16"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="10"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="14"/>
+      <c r="B72" s="16"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="10"/>
-      <c r="B73" s="12"/>
+      <c r="A73" s="14"/>
+      <c r="B73" s="16"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="10"/>
-      <c r="B74" s="12"/>
+      <c r="A74" s="14"/>
+      <c r="B74" s="16"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="10"/>
-      <c r="B75" s="12"/>
+      <c r="A75" s="14"/>
+      <c r="B75" s="16"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="10"/>
-      <c r="B76" s="12"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="16"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="10"/>
-      <c r="B77" s="12"/>
+      <c r="A77" s="14"/>
+      <c r="B77" s="16"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="10"/>
-      <c r="B78" s="12"/>
+      <c r="A78" s="14"/>
+      <c r="B78" s="16"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="10"/>
-      <c r="B79" s="12"/>
+      <c r="A79" s="14"/>
+      <c r="B79" s="16"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="10"/>
-      <c r="B80" s="12"/>
+      <c r="A80" s="14"/>
+      <c r="B80" s="16"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="10"/>
-      <c r="B81" s="12"/>
+      <c r="A81" s="14"/>
+      <c r="B81" s="16"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="10"/>
-      <c r="B82" s="12"/>
+      <c r="A82" s="14"/>
+      <c r="B82" s="16"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="10"/>
-      <c r="B83" s="12"/>
+      <c r="A83" s="14"/>
+      <c r="B83" s="16"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="10"/>
-      <c r="B84" s="12"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="16"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="10"/>
-      <c r="B85" s="12"/>
+      <c r="A85" s="14"/>
+      <c r="B85" s="16"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="10"/>
-      <c r="B86" s="12"/>
+      <c r="A86" s="14"/>
+      <c r="B86" s="16"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="10"/>
-      <c r="B87" s="12"/>
+      <c r="A87" s="14"/>
+      <c r="B87" s="16"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="10"/>
-      <c r="B88" s="12"/>
+      <c r="A88" s="14"/>
+      <c r="B88" s="16"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="10"/>
-      <c r="B89" s="12"/>
+      <c r="A89" s="14"/>
+      <c r="B89" s="16"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="10"/>
-      <c r="B90" s="12"/>
+      <c r="A90" s="14"/>
+      <c r="B90" s="16"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="10"/>
-      <c r="B91" s="12"/>
+      <c r="A91" s="14"/>
+      <c r="B91" s="16"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="10"/>
-      <c r="B92" s="12"/>
+      <c r="A92" s="14"/>
+      <c r="B92" s="16"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="10"/>
-      <c r="B93" s="12"/>
+      <c r="A93" s="14"/>
+      <c r="B93" s="16"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="10"/>
-      <c r="B94" s="12"/>
+      <c r="A94" s="14"/>
+      <c r="B94" s="16"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="10"/>
-      <c r="B95" s="12"/>
+      <c r="A95" s="14"/>
+      <c r="B95" s="16"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="10"/>
-      <c r="B96" s="12"/>
+      <c r="A96" s="14"/>
+      <c r="B96" s="16"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="10"/>
-      <c r="B97" s="12"/>
+      <c r="A97" s="14"/>
+      <c r="B97" s="16"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="10"/>
-      <c r="B98" s="12"/>
+      <c r="A98" s="14"/>
+      <c r="B98" s="16"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="10"/>
-      <c r="B99" s="12"/>
+      <c r="A99" s="14"/>
+      <c r="B99" s="16"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="10"/>
-      <c r="B100" s="12"/>
+      <c r="A100" s="14"/>
+      <c r="B100" s="16"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="A101" s="10"/>
-      <c r="B101" s="12"/>
+      <c r="A101" s="14"/>
+      <c r="B101" s="16"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="A102" s="10"/>
-      <c r="B102" s="12"/>
+      <c r="A102" s="14"/>
+      <c r="B102" s="16"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="A103" s="10"/>
-      <c r="B103" s="12"/>
+      <c r="A103" s="14"/>
+      <c r="B103" s="16"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="A104" s="10"/>
-      <c r="B104" s="12"/>
+      <c r="A104" s="14"/>
+      <c r="B104" s="16"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="A105" s="10"/>
-      <c r="B105" s="12"/>
+      <c r="A105" s="14"/>
+      <c r="B105" s="16"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="A106" s="10"/>
-      <c r="B106" s="12"/>
+      <c r="A106" s="14"/>
+      <c r="B106" s="16"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="A107" s="10"/>
-      <c r="B107" s="12"/>
+      <c r="A107" s="14"/>
+      <c r="B107" s="16"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="A108" s="10"/>
-      <c r="B108" s="12"/>
+      <c r="A108" s="14"/>
+      <c r="B108" s="16"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="A109" s="10"/>
-      <c r="B109" s="12"/>
+      <c r="A109" s="14"/>
+      <c r="B109" s="16"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="A110" s="10"/>
-      <c r="B110" s="12"/>
+      <c r="A110" s="14"/>
+      <c r="B110" s="16"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="A111" s="10"/>
-      <c r="B111" s="12"/>
+      <c r="A111" s="14"/>
+      <c r="B111" s="16"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="A112" s="10"/>
-      <c r="B112" s="12"/>
+      <c r="A112" s="14"/>
+      <c r="B112" s="16"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="A113" s="10"/>
-      <c r="B113" s="12"/>
+      <c r="A113" s="14"/>
+      <c r="B113" s="16"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="A114" s="10"/>
-      <c r="B114" s="12"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="16"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="A115" s="10"/>
-      <c r="B115" s="12"/>
+      <c r="A115" s="14"/>
+      <c r="B115" s="16"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="A116" s="10"/>
-      <c r="B116" s="12"/>
+      <c r="A116" s="14"/>
+      <c r="B116" s="16"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="A117" s="10"/>
-      <c r="B117" s="12"/>
+      <c r="A117" s="14"/>
+      <c r="B117" s="16"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="A118" s="10"/>
-      <c r="B118" s="12"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="16"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="A119" s="10"/>
-      <c r="B119" s="12"/>
+      <c r="A119" s="14"/>
+      <c r="B119" s="16"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="A120" s="10"/>
-      <c r="B120" s="12"/>
+      <c r="A120" s="14"/>
+      <c r="B120" s="16"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="A121" s="10"/>
-      <c r="B121" s="12"/>
+      <c r="A121" s="14"/>
+      <c r="B121" s="16"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="A122" s="10"/>
-      <c r="B122" s="12"/>
+      <c r="A122" s="14"/>
+      <c r="B122" s="16"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="A123" s="10"/>
-      <c r="B123" s="12"/>
+      <c r="A123" s="14"/>
+      <c r="B123" s="16"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="A124" s="10"/>
-      <c r="B124" s="12"/>
+      <c r="A124" s="14"/>
+      <c r="B124" s="16"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="A125" s="10"/>
-      <c r="B125" s="12"/>
+      <c r="A125" s="14"/>
+      <c r="B125" s="16"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="A126" s="10"/>
-      <c r="B126" s="12"/>
+      <c r="A126" s="14"/>
+      <c r="B126" s="16"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="A127" s="10"/>
-      <c r="B127" s="12"/>
+      <c r="A127" s="14"/>
+      <c r="B127" s="16"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="A128" s="10"/>
-      <c r="B128" s="12"/>
+      <c r="A128" s="14"/>
+      <c r="B128" s="16"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="A129" s="10"/>
-      <c r="B129" s="12"/>
+      <c r="A129" s="14"/>
+      <c r="B129" s="16"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="A130" s="10"/>
-      <c r="B130" s="12"/>
+      <c r="A130" s="14"/>
+      <c r="B130" s="16"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="A131" s="10"/>
-      <c r="B131" s="12"/>
+      <c r="A131" s="14"/>
+      <c r="B131" s="16"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="A132" s="10"/>
-      <c r="B132" s="12"/>
+      <c r="A132" s="14"/>
+      <c r="B132" s="16"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="A133" s="10"/>
-      <c r="B133" s="12"/>
+      <c r="A133" s="14"/>
+      <c r="B133" s="16"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="A134" s="10"/>
-      <c r="B134" s="12"/>
+      <c r="A134" s="14"/>
+      <c r="B134" s="16"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="A135" s="10"/>
-      <c r="B135" s="12"/>
+      <c r="A135" s="14"/>
+      <c r="B135" s="16"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="A136" s="10"/>
-      <c r="B136" s="12"/>
+      <c r="A136" s="14"/>
+      <c r="B136" s="16"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="A137" s="10"/>
-      <c r="B137" s="12"/>
+      <c r="A137" s="14"/>
+      <c r="B137" s="16"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="A138" s="10"/>
-      <c r="B138" s="12"/>
+      <c r="A138" s="14"/>
+      <c r="B138" s="16"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="A139" s="10"/>
-      <c r="B139" s="12"/>
+      <c r="A139" s="14"/>
+      <c r="B139" s="16"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="A140" s="10"/>
-      <c r="B140" s="12"/>
+      <c r="A140" s="14"/>
+      <c r="B140" s="16"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="A141" s="10"/>
-      <c r="B141" s="12"/>
+      <c r="A141" s="14"/>
+      <c r="B141" s="16"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="A142" s="10"/>
-      <c r="B142" s="12"/>
+      <c r="A142" s="14"/>
+      <c r="B142" s="16"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="A143" s="10"/>
-      <c r="B143" s="12"/>
+      <c r="A143" s="14"/>
+      <c r="B143" s="16"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="A144" s="10"/>
-      <c r="B144" s="12"/>
+      <c r="A144" s="14"/>
+      <c r="B144" s="16"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="A145" s="10"/>
-      <c r="B145" s="12"/>
+      <c r="A145" s="14"/>
+      <c r="B145" s="16"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="A146" s="10"/>
-      <c r="B146" s="12"/>
+      <c r="A146" s="14"/>
+      <c r="B146" s="16"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="A147" s="10"/>
-      <c r="B147" s="12"/>
+      <c r="A147" s="14"/>
+      <c r="B147" s="16"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="A148" s="10"/>
-      <c r="B148" s="12"/>
+      <c r="A148" s="14"/>
+      <c r="B148" s="16"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="A149" s="10"/>
-      <c r="B149" s="12"/>
+      <c r="A149" s="14"/>
+      <c r="B149" s="16"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="A150" s="10"/>
-      <c r="B150" s="12"/>
+      <c r="A150" s="14"/>
+      <c r="B150" s="16"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="A151" s="10"/>
-      <c r="B151" s="12"/>
+      <c r="A151" s="14"/>
+      <c r="B151" s="16"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="A152" s="10"/>
-      <c r="B152" s="12"/>
+      <c r="A152" s="14"/>
+      <c r="B152" s="16"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="A153" s="10"/>
-      <c r="B153" s="12"/>
+      <c r="A153" s="14"/>
+      <c r="B153" s="16"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="A154" s="10"/>
-      <c r="B154" s="12"/>
+      <c r="A154" s="14"/>
+      <c r="B154" s="16"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="A155" s="10"/>
-      <c r="B155" s="12"/>
+      <c r="A155" s="14"/>
+      <c r="B155" s="16"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="A156" s="10"/>
-      <c r="B156" s="12"/>
+      <c r="A156" s="14"/>
+      <c r="B156" s="16"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="A157" s="10"/>
-      <c r="B157" s="12"/>
+      <c r="A157" s="14"/>
+      <c r="B157" s="16"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="A158" s="10"/>
-      <c r="B158" s="12"/>
+      <c r="A158" s="14"/>
+      <c r="B158" s="16"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="A159" s="10"/>
-      <c r="B159" s="12"/>
+      <c r="A159" s="14"/>
+      <c r="B159" s="16"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="A160" s="10"/>
-      <c r="B160" s="12"/>
+      <c r="A160" s="14"/>
+      <c r="B160" s="16"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="A161" s="10"/>
-      <c r="B161" s="12"/>
+      <c r="A161" s="14"/>
+      <c r="B161" s="16"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="A162" s="10"/>
-      <c r="B162" s="12"/>
+      <c r="A162" s="14"/>
+      <c r="B162" s="16"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="A163" s="10"/>
-      <c r="B163" s="12"/>
+      <c r="A163" s="14"/>
+      <c r="B163" s="16"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="A164" s="10"/>
-      <c r="B164" s="12"/>
+      <c r="A164" s="14"/>
+      <c r="B164" s="16"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="A165" s="10"/>
-      <c r="B165" s="12"/>
+      <c r="A165" s="14"/>
+      <c r="B165" s="16"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="A166" s="10"/>
-      <c r="B166" s="12"/>
+      <c r="A166" s="14"/>
+      <c r="B166" s="16"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="A167" s="10"/>
-      <c r="B167" s="12"/>
+      <c r="A167" s="14"/>
+      <c r="B167" s="16"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="A168" s="10"/>
-      <c r="B168" s="12"/>
+      <c r="A168" s="14"/>
+      <c r="B168" s="16"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="A169" s="10"/>
-      <c r="B169" s="12"/>
+      <c r="A169" s="14"/>
+      <c r="B169" s="16"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="A170" s="10"/>
-      <c r="B170" s="12"/>
+      <c r="A170" s="14"/>
+      <c r="B170" s="16"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="A171" s="10"/>
-      <c r="B171" s="12"/>
+      <c r="A171" s="14"/>
+      <c r="B171" s="16"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="A172" s="10"/>
-      <c r="B172" s="12"/>
+      <c r="A172" s="14"/>
+      <c r="B172" s="16"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="A173" s="10"/>
-      <c r="B173" s="12"/>
+      <c r="A173" s="14"/>
+      <c r="B173" s="16"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="A174" s="10"/>
-      <c r="B174" s="12"/>
+      <c r="A174" s="14"/>
+      <c r="B174" s="16"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="A175" s="10"/>
-      <c r="B175" s="12"/>
+      <c r="A175" s="14"/>
+      <c r="B175" s="16"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="A176" s="10"/>
-      <c r="B176" s="12"/>
+      <c r="A176" s="14"/>
+      <c r="B176" s="16"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="A177" s="10"/>
-      <c r="B177" s="12"/>
+      <c r="A177" s="14"/>
+      <c r="B177" s="16"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="A178" s="10"/>
-      <c r="B178" s="12"/>
+      <c r="A178" s="14"/>
+      <c r="B178" s="16"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="A179" s="10"/>
-      <c r="B179" s="12"/>
+      <c r="A179" s="14"/>
+      <c r="B179" s="16"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="A180" s="10"/>
-      <c r="B180" s="12"/>
+      <c r="A180" s="14"/>
+      <c r="B180" s="16"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="A181" s="10"/>
-      <c r="B181" s="12"/>
+      <c r="A181" s="14"/>
+      <c r="B181" s="16"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="A182" s="10"/>
-      <c r="B182" s="12"/>
+      <c r="A182" s="14"/>
+      <c r="B182" s="16"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="A183" s="10"/>
-      <c r="B183" s="12"/>
+      <c r="A183" s="14"/>
+      <c r="B183" s="16"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="A184" s="10"/>
-      <c r="B184" s="12"/>
+      <c r="A184" s="14"/>
+      <c r="B184" s="16"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="A185" s="10"/>
-      <c r="B185" s="12"/>
+      <c r="A185" s="14"/>
+      <c r="B185" s="16"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="A186" s="10"/>
-      <c r="B186" s="12"/>
+      <c r="A186" s="14"/>
+      <c r="B186" s="16"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="A187" s="10"/>
-      <c r="B187" s="12"/>
+      <c r="A187" s="14"/>
+      <c r="B187" s="16"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="A188" s="10"/>
-      <c r="B188" s="12"/>
+      <c r="A188" s="14"/>
+      <c r="B188" s="16"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="A189" s="10"/>
-      <c r="B189" s="12"/>
+      <c r="A189" s="14"/>
+      <c r="B189" s="16"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="A190" s="10"/>
-      <c r="B190" s="12"/>
+      <c r="A190" s="14"/>
+      <c r="B190" s="16"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="A191" s="10"/>
-      <c r="B191" s="12"/>
+      <c r="A191" s="14"/>
+      <c r="B191" s="16"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="A192" s="10"/>
-      <c r="B192" s="12"/>
+      <c r="A192" s="14"/>
+      <c r="B192" s="16"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="A193" s="10"/>
-      <c r="B193" s="12"/>
+      <c r="A193" s="14"/>
+      <c r="B193" s="16"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="A194" s="10"/>
-      <c r="B194" s="12"/>
+      <c r="A194" s="14"/>
+      <c r="B194" s="16"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="A195" s="10"/>
-      <c r="B195" s="12"/>
+      <c r="A195" s="14"/>
+      <c r="B195" s="16"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="A196" s="10"/>
-      <c r="B196" s="12"/>
+      <c r="A196" s="14"/>
+      <c r="B196" s="16"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="10"/>
-      <c r="B197" s="12"/>
+      <c r="A197" s="14"/>
+      <c r="B197" s="16"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="A198" s="10"/>
-      <c r="B198" s="12"/>
+      <c r="A198" s="14"/>
+      <c r="B198" s="16"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="A199" s="10"/>
-      <c r="B199" s="12"/>
+      <c r="A199" s="14"/>
+      <c r="B199" s="16"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="A200" s="10"/>
-      <c r="B200" s="12"/>
+      <c r="A200" s="14"/>
+      <c r="B200" s="16"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="A201" s="10"/>
-      <c r="B201" s="12"/>
+      <c r="A201" s="14"/>
+      <c r="B201" s="16"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="A202" s="10"/>
-      <c r="B202" s="12"/>
+      <c r="A202" s="14"/>
+      <c r="B202" s="16"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="A203" s="10"/>
-      <c r="B203" s="12"/>
+      <c r="A203" s="14"/>
+      <c r="B203" s="16"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="A204" s="10"/>
-      <c r="B204" s="12"/>
+      <c r="A204" s="14"/>
+      <c r="B204" s="16"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="A205" s="10"/>
-      <c r="B205" s="12"/>
+      <c r="A205" s="14"/>
+      <c r="B205" s="16"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="A206" s="10"/>
-      <c r="B206" s="12"/>
+      <c r="A206" s="14"/>
+      <c r="B206" s="16"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="A207" s="10"/>
-      <c r="B207" s="12"/>
+      <c r="A207" s="14"/>
+      <c r="B207" s="16"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="10"/>
-      <c r="B208" s="12"/>
+      <c r="A208" s="14"/>
+      <c r="B208" s="16"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="10"/>
-      <c r="B209" s="12"/>
+      <c r="A209" s="14"/>
+      <c r="B209" s="16"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="A210" s="10"/>
-      <c r="B210" s="12"/>
+      <c r="A210" s="14"/>
+      <c r="B210" s="16"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="A211" s="10"/>
-      <c r="B211" s="12"/>
+      <c r="A211" s="14"/>
+      <c r="B211" s="16"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="A212" s="10"/>
-      <c r="B212" s="12"/>
+      <c r="A212" s="14"/>
+      <c r="B212" s="16"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="A213" s="10"/>
-      <c r="B213" s="12"/>
+      <c r="A213" s="14"/>
+      <c r="B213" s="16"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="A214" s="10"/>
-      <c r="B214" s="12"/>
+      <c r="A214" s="14"/>
+      <c r="B214" s="16"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="A215" s="10"/>
-      <c r="B215" s="12"/>
+      <c r="A215" s="14"/>
+      <c r="B215" s="16"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="A216" s="10"/>
-      <c r="B216" s="12"/>
+      <c r="A216" s="14"/>
+      <c r="B216" s="16"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="A217" s="10"/>
-      <c r="B217" s="12"/>
+      <c r="A217" s="14"/>
+      <c r="B217" s="16"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="A218" s="10"/>
-      <c r="B218" s="12"/>
+      <c r="A218" s="14"/>
+      <c r="B218" s="16"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="A219" s="10"/>
-      <c r="B219" s="12"/>
+      <c r="A219" s="14"/>
+      <c r="B219" s="16"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="A220" s="10"/>
-      <c r="B220" s="12"/>
+      <c r="A220" s="14"/>
+      <c r="B220" s="16"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -10843,7 +11017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10852,39 +11026,48 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="36.63"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>41</v>
+      <c r="A1" s="8" t="s">
+        <v>46</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>25</v>
+      <c r="B1" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>42</v>
+      <c r="A2" s="8" t="s">
+        <v>47</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>43</v>
+      <c r="B2" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>44</v>
+      <c r="A3" s="8" t="s">
+        <v>49</v>
       </c>
-      <c r="B3" s="13">
-        <v>1234.0</v>
+      <c r="B3" s="17" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13">
-        <v>1234.0</v>
+      <c r="A4" s="8" t="s">
+        <v>51</v>
       </c>
+      <c r="B4" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>43</v>
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -10892,7 +11075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -10907,67 +11090,67 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="13" t="s">
-        <v>45</v>
+      <c r="A1" s="8" t="s">
+        <v>55</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>46</v>
+      <c r="B1" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="s">
-        <v>47</v>
+      <c r="A2" s="8" t="s">
+        <v>57</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>47</v>
+      <c r="B2" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="s">
-        <v>48</v>
+      <c r="A3" s="8" t="s">
+        <v>58</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>48</v>
+      <c r="B3" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>49</v>
+      <c r="A4" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>49</v>
+      <c r="B4" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>50</v>
+      <c r="A5" s="8" t="s">
+        <v>60</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>50</v>
+      <c r="B5" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>51</v>
+      <c r="A6" s="8" t="s">
+        <v>61</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>51</v>
+      <c r="B6" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>52</v>
+      <c r="A7" s="8" t="s">
+        <v>62</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>52</v>
+      <c r="B7" s="8" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="s">
-        <v>53</v>
+      <c r="A8" s="8" t="s">
+        <v>63</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>53</v>
+      <c r="B8" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>